<commit_message>
Native aangemaakt; Tabs mosque, prayer en favorite aangemaakt, menu in action bar aangemaakt, xml files voor meerdere talen: NL,DE,FR
icon set toegevoegd (XHDPI,HDPI,MDPI)

Issues momenteel:
- App crasht omdat google maps niet geladen wordt met de nieuwe API V2
- Tabs krijgen geen icons

Nog te doen:
- Logo toevoegen
- TableLayout voor favorite tab
- TableLayout met checkbox voor prayer tab
- Settings Activity aanmaken
-Strings XML updaten en alle gehard coded strings in strings xml zetten
ook voor de verschillende talen
</commit_message>
<xml_diff>
--- a/Documentatie/PlanningTemplate.xlsx
+++ b/Documentatie/PlanningTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Deadline</t>
   </si>
@@ -46,6 +46,42 @@
   </si>
   <si>
     <t>To Do (E-F)</t>
+  </si>
+  <si>
+    <t>Mockups</t>
+  </si>
+  <si>
+    <t>Nabil</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Native App</t>
+  </si>
+  <si>
+    <t>Logo Maken</t>
+  </si>
+  <si>
+    <t>Moodboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI </t>
+  </si>
+  <si>
+    <t>DB schema</t>
+  </si>
+  <si>
+    <t>Website Draft</t>
+  </si>
+  <si>
+    <t>Osamah</t>
+  </si>
+  <si>
+    <t>Code schrijven</t>
+  </si>
+  <si>
+    <t>Website</t>
   </si>
 </sst>
 </file>
@@ -162,7 +198,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -170,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -188,10 +225,15 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -519,21 +561,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.375" customWidth="1"/>
     <col min="6" max="6" width="24.5" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -544,7 +586,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="20">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -567,11 +609,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7">
+        <v>41261</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5">
@@ -579,11 +629,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7">
+        <v>41261</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5">
@@ -591,11 +649,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
+        <v>41264</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5">
@@ -603,11 +667,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7">
+        <v>41264</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5">
@@ -615,11 +685,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7">
+        <v>41273</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5">
@@ -627,11 +705,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7">
+        <v>41261</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5">
@@ -639,11 +723,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7">
+        <v>41261</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5">
@@ -651,11 +741,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7">
+        <v>41264</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5">
@@ -663,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -675,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -687,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -699,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -711,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -723,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -735,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -747,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -759,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -771,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -783,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -795,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -807,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -819,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -831,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -843,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -855,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -867,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -879,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -891,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -903,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -915,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -927,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -939,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -951,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -963,7 +1061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -975,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -987,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -999,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1011,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1023,7 +1121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1035,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1047,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1059,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1071,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1083,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1095,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1107,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1119,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1131,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1143,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1155,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1167,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1179,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -1191,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1203,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>4</v>
       </c>
@@ -1211,7 +1309,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="6">
         <f t="shared" ref="D56:F56" si="2">SUM(D3:D55)</f>
-        <v>0</v>
+        <v>330109</v>
       </c>
       <c r="E56" s="6">
         <f t="shared" si="2"/>

</xml_diff>